<commit_message>
refactor for less code duplication between session and person import
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX_People.xlsx
+++ b/sample data/LingMetaX_People.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>full_name</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Woody</t>
   </si>
   <si>
-    <t>maile</t>
-  </si>
-  <si>
     <t>City of London Freemen's School</t>
   </si>
   <si>
@@ -84,6 +81,12 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Joe Strummer</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,32 +466,35 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>1952</v>
       </c>
       <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can replace existing when importing people
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX_People.xlsx
+++ b/sample data/LingMetaX_People.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>full_name</t>
   </si>
@@ -87,13 +87,22 @@
   </si>
   <si>
     <t>Joe Strummer</t>
+  </si>
+  <si>
+    <t>Vince White</t>
+  </si>
+  <si>
+    <t>University College London</t>
+  </si>
+  <si>
+    <t>lead guitar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +114,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,14 +144,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +517,31 @@
         <v>18</v>
       </c>
     </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>1960</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" tooltip="University College London" display="https://en.wikipedia.org/wiki/University_College_London"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Import language list for person
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX_People.xlsx
+++ b/sample data/LingMetaX_People.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>full_name</t>
   </si>
@@ -96,13 +96,22 @@
   </si>
   <si>
     <t>lead guitar</t>
+  </si>
+  <si>
+    <t>qab</t>
+  </si>
+  <si>
+    <t>French, etr;Español;qac</t>
+  </si>
+  <si>
+    <t>London</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +135,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -148,10 +163,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -436,10 +454,15 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -476,13 +499,13 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -508,13 +531,16 @@
         <v>17</v>
       </c>
       <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
         <v>18</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -535,6 +561,12 @@
       </c>
       <c r="I3" t="s">
         <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On person import, catch languages we can't make sense of
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX_People.xlsx
+++ b/sample data/LingMetaX_People.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>full_name</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>London</t>
+  </si>
+  <si>
+    <t>Englishes</t>
+  </si>
+  <si>
+    <t>fr;foo,ru,spa</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,10 +569,13 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="K3" t="s">
         <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sanitize custom field names on spreadsheet import
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX_People.xlsx
+++ b/sample data/LingMetaX_People.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\lameta\sample data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF070C5D-8020-47D2-A67C-D5F98E1AF97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>full_name</t>
   </si>
@@ -111,12 +112,18 @@
   </si>
   <si>
     <t>fr;foo,ru,spa</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>custom column with spaces</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,11 +463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +477,7 @@
     <col min="14" max="14" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,8 +520,11 @@
       <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -548,8 +558,11 @@
       <c r="N2" t="s">
         <v>25</v>
       </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -580,7 +593,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" tooltip="University College London" display="https://en.wikipedia.org/wiki/University_College_London"/>
+    <hyperlink ref="F3" r:id="rId1" tooltip="University College London" display="https://en.wikipedia.org/wiki/University_College_London" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>